<commit_message>
updating AXP model, still long, still not a solicitation to buy/sell
</commit_message>
<xml_diff>
--- a/AXP.xlsx
+++ b/AXP.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameelbrannon/Dropbox/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6118A316-C260-1346-B592-AB9C9738DD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB302CAA-462B-B84C-BA8D-F22089996C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="500" windowWidth="44280" windowHeight="24540" activeTab="1" xr2:uid="{6D904A83-089B-B64C-BA83-931F47940392}"/>
+    <workbookView xWindow="520" yWindow="500" windowWidth="44280" windowHeight="24540" activeTab="1" xr2:uid="{6D904A83-089B-B64C-BA83-931F47940392}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
     <sheet name="Main" sheetId="2" r:id="rId2"/>
+    <sheet name="data analysis" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -249,6 +250,39 @@
     <author>Brannon, Jameel A.</author>
   </authors>
   <commentList>
+    <comment ref="M5" authorId="0" shapeId="0" xr:uid="{794D9F24-EDB6-154D-9B65-D3A18704CE7E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Brannon, Jameel A.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>this was the rule when I was in college, seems this rule has become abandoned???</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C9" authorId="0" shapeId="0" xr:uid="{980D71CE-F35E-DC40-9DC6-F9C759B16D00}">
       <text>
         <r>
@@ -279,6 +313,93 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Manages relationships with merchants </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{ECD74276-A9C4-1445-AECE-B0EB6F2C19E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Brannon, Jameel A.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">If everytime i buy something I can gain rewards (points/cash back) -- then why ever buy an item in cash?
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If you hold a card where you can recieve a return (points, etc) when it's used, and you instead use cash --- should it be considered an intrinsic negative return on your monthly spending?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K12" authorId="0" shapeId="0" xr:uid="{50DC359C-CF82-B240-9E22-2FDAD52C5995}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Brannon, Jameel A.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">unemployement + LFPR
+</t>
         </r>
       </text>
     </comment>
@@ -419,12 +540,45 @@
         </r>
       </text>
     </comment>
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{FE98EAD5-C64E-D644-BEEF-0C3F85F3725B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Brannon, Jameel A.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Grew 2.6% in q3'22. in q2'22 GDP shrunk 0.6%</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="188">
   <si>
     <t>Q119</t>
   </si>
@@ -949,6 +1103,45 @@
   </si>
   <si>
     <t>EV/E 21</t>
+  </si>
+  <si>
+    <t>Catalyst</t>
+  </si>
+  <si>
+    <t>Cons</t>
+  </si>
+  <si>
+    <t>Massive layoffs</t>
+  </si>
+  <si>
+    <t>Inflation --&gt; Taking up descretionary income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recession </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recession = 2 negative q's of GDP growth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unemployment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDP </t>
+  </si>
+  <si>
+    <t>Fed Balance Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand strength </t>
+  </si>
+  <si>
+    <t>Holidays</t>
+  </si>
+  <si>
+    <t>Collge Football Travel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Cup Travel </t>
   </si>
 </sst>
 </file>
@@ -960,7 +1153,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="170" formatCode="0.0\x"/>
+    <numFmt numFmtId="167" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -1269,7 +1462,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1364,7 +1557,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1391,7 +1584,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1419,6 +1612,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1856,11 +2058,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{707E2F29-3D1E-DF44-822A-F1331C631B30}">
   <dimension ref="B2:EV116"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="H13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2032,7 +2234,7 @@
         <v>6181</v>
       </c>
       <c r="F3" s="3">
-        <f>+AD3-SUM(C3:E3)</f>
+        <f t="shared" ref="F3:F30" si="1">+AD3-SUM(C3:E3)</f>
         <v>6457</v>
       </c>
       <c r="G3" s="3">
@@ -2045,7 +2247,7 @@
         <v>6566</v>
       </c>
       <c r="J3" s="3">
-        <f>+AE3-SUM(G3:I3)</f>
+        <f t="shared" ref="J3:J30" si="2">+AE3-SUM(G3:I3)</f>
         <v>6829</v>
       </c>
       <c r="K3" s="3">
@@ -2058,7 +2260,7 @@
         <v>4999</v>
       </c>
       <c r="N3" s="3">
-        <f>+AF3-SUM(K3:M3)</f>
+        <f t="shared" ref="N3:N30" si="3">+AF3-SUM(K3:M3)</f>
         <v>5549</v>
       </c>
       <c r="O3" s="3">
@@ -2071,7 +2273,7 @@
         <v>6676</v>
       </c>
       <c r="R3" s="3">
-        <f>+AG3-SUM(O3:Q3)</f>
+        <f t="shared" ref="R3:R30" si="4">+AG3-SUM(O3:Q3)</f>
         <v>7482</v>
       </c>
       <c r="S3" s="3">
@@ -2112,7 +2314,7 @@
         <v>25727</v>
       </c>
       <c r="AH3" s="3">
-        <f>+SUM(S3:V3)</f>
+        <f t="shared" ref="AH3:AH30" si="5">+SUM(S3:V3)</f>
         <v>30130.82</v>
       </c>
     </row>
@@ -2130,7 +2332,7 @@
         <v>870</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4:F32" si="1">+AD4-SUM(C4:E4)</f>
+        <f t="shared" si="1"/>
         <v>897</v>
       </c>
       <c r="G4" s="3">
@@ -2143,7 +2345,7 @@
         <v>1033</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J32" si="2">+AE4-SUM(G4:I4)</f>
+        <f t="shared" si="2"/>
         <v>1077</v>
       </c>
       <c r="K4" s="3">
@@ -2156,7 +2358,7 @@
         <v>1191</v>
       </c>
       <c r="N4" s="3">
-        <f t="shared" ref="N4:N32" si="3">+AF4-SUM(K4:M4)</f>
+        <f t="shared" si="3"/>
         <v>1222</v>
       </c>
       <c r="O4" s="3">
@@ -2169,7 +2371,7 @@
         <v>1312</v>
       </c>
       <c r="R4" s="3">
-        <f t="shared" ref="R4:R32" si="4">+AG4-SUM(O4:Q4)</f>
+        <f t="shared" si="4"/>
         <v>1344</v>
       </c>
       <c r="S4" s="3">
@@ -2182,7 +2384,7 @@
         <v>1541</v>
       </c>
       <c r="V4" s="3">
-        <f t="shared" ref="V4:V6" si="5">+R4*1.01</f>
+        <f>+R4*1.01</f>
         <v>1357.44</v>
       </c>
       <c r="Z4" s="3">
@@ -2210,7 +2412,7 @@
         <v>5195</v>
       </c>
       <c r="AH4" s="3">
-        <f t="shared" ref="AH4:AH32" si="6">+SUM(S4:V4)</f>
+        <f t="shared" si="5"/>
         <v>5802.4400000000005</v>
       </c>
     </row>
@@ -2280,7 +2482,7 @@
         <v>1169</v>
       </c>
       <c r="V5" s="3">
-        <f t="shared" si="5"/>
+        <f>+R5*1.01</f>
         <v>686.8</v>
       </c>
       <c r="Z5" s="3">
@@ -2308,7 +2510,7 @@
         <v>2392</v>
       </c>
       <c r="AH5" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>4026.8</v>
       </c>
     </row>
@@ -2378,7 +2580,7 @@
         <v>420</v>
       </c>
       <c r="V6" s="3">
-        <f t="shared" si="5"/>
+        <f>+R6*1.01</f>
         <v>536.31000000000006</v>
       </c>
       <c r="Z6" s="3">
@@ -2406,7 +2608,7 @@
         <v>1316</v>
       </c>
       <c r="AH6" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1744.31</v>
       </c>
     </row>
@@ -2496,39 +2698,39 @@
       </c>
       <c r="X7" s="13"/>
       <c r="Z7" s="5">
-        <f t="shared" ref="Z7:AG7" si="7">+SUM(Z3:Z6)</f>
+        <f t="shared" ref="Z7:AG7" si="6">+SUM(Z3:Z6)</f>
         <v>28716</v>
       </c>
       <c r="AA7" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>26896</v>
       </c>
       <c r="AB7" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>29659</v>
       </c>
       <c r="AC7" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>30427</v>
       </c>
       <c r="AD7" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>32675</v>
       </c>
       <c r="AE7" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>34936</v>
       </c>
       <c r="AF7" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>28102</v>
       </c>
       <c r="AG7" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>34630</v>
       </c>
       <c r="AH7" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>41704.369999999995</v>
       </c>
     </row>
@@ -2626,7 +2828,7 @@
         <v>8850</v>
       </c>
       <c r="AH8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>11265.719683002368</v>
       </c>
     </row>
@@ -2696,7 +2898,7 @@
         <v>27</v>
       </c>
       <c r="V9" s="3">
-        <f t="shared" ref="V9:V10" si="8">+V$7*(U9/U$7)</f>
+        <f>+V$7*(U9/U$7)</f>
         <v>24.932500455456367</v>
       </c>
       <c r="Z9" s="3">
@@ -2724,7 +2926,7 @@
         <v>83</v>
       </c>
       <c r="AH9" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>86.932500455456363</v>
       </c>
     </row>
@@ -2794,7 +2996,7 @@
         <v>183</v>
       </c>
       <c r="V10" s="3">
-        <f t="shared" si="8"/>
+        <f>+V$7*(U10/U$7)</f>
         <v>168.98694753142647</v>
       </c>
       <c r="Z10" s="3">
@@ -2822,7 +3024,7 @@
         <v>100</v>
       </c>
       <c r="AH10" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>455.98694753142649</v>
       </c>
     </row>
@@ -2912,39 +3114,39 @@
       </c>
       <c r="X11" s="13"/>
       <c r="Z11" s="5">
-        <f t="shared" ref="Z11:AG11" si="9">+SUM(Z8:Z10)</f>
+        <f t="shared" ref="Z11:AG11" si="7">+SUM(Z8:Z10)</f>
         <v>7179</v>
       </c>
       <c r="AA11" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>7545</v>
       </c>
       <c r="AB11" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>7484</v>
       </c>
       <c r="AC11" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>8563</v>
       </c>
       <c r="AD11" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>10606</v>
       </c>
       <c r="AE11" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>12084</v>
       </c>
       <c r="AF11" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>10083</v>
       </c>
       <c r="AG11" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>9033</v>
       </c>
       <c r="AH11" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>11808.63913098925</v>
       </c>
     </row>
@@ -3042,7 +3244,7 @@
         <v>458</v>
       </c>
       <c r="AH12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1155.3074148296591</v>
       </c>
     </row>
@@ -3112,7 +3314,7 @@
         <v>356</v>
       </c>
       <c r="V13" s="3">
-        <f t="shared" ref="V13" si="10">+V$11*(U13/U$11)</f>
+        <f>+V$11*(U13/U$11)</f>
         <v>328.73963563490611</v>
       </c>
       <c r="Z13" s="3">
@@ -3140,7 +3342,7 @@
         <v>825</v>
       </c>
       <c r="AH13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1135.7396356349061</v>
       </c>
     </row>
@@ -3229,39 +3431,39 @@
         <v>735.04705046456536</v>
       </c>
       <c r="Z14" s="3">
-        <f t="shared" ref="Z14:AG14" si="11">+SUM(Z12:Z13)</f>
+        <f t="shared" ref="Z14:AG14" si="8">+SUM(Z12:Z13)</f>
         <v>1707</v>
       </c>
       <c r="AA14" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>1623</v>
       </c>
       <c r="AB14" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>1705</v>
       </c>
       <c r="AC14" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>2112</v>
       </c>
       <c r="AD14" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>2943</v>
       </c>
       <c r="AE14" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>3464</v>
       </c>
       <c r="AF14" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>2098</v>
       </c>
       <c r="AG14" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>1283</v>
       </c>
       <c r="AH14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2291.0470504645655</v>
       </c>
     </row>
@@ -3351,39 +3553,39 @@
       </c>
       <c r="X15" s="13"/>
       <c r="Z15" s="5">
-        <f t="shared" ref="Z15:AG15" si="12">+Z11-Z14</f>
+        <f t="shared" ref="Z15:AG15" si="9">+Z11-Z14</f>
         <v>5472</v>
       </c>
       <c r="AA15" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>5922</v>
       </c>
       <c r="AB15" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>5779</v>
       </c>
       <c r="AC15" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>6451</v>
       </c>
       <c r="AD15" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>7663</v>
       </c>
       <c r="AE15" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>8620</v>
       </c>
       <c r="AF15" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>7985</v>
       </c>
       <c r="AG15" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>7750</v>
       </c>
       <c r="AH15" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>9517.592080524686</v>
       </c>
     </row>
@@ -3473,75 +3675,75 @@
       </c>
       <c r="X16" s="13"/>
       <c r="Z16" s="5">
-        <f t="shared" ref="Z16:AG16" si="13">+Z7+Z15</f>
+        <f t="shared" ref="Z16:AG16" si="10">+Z7+Z15</f>
         <v>34188</v>
       </c>
       <c r="AA16" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>32818</v>
       </c>
       <c r="AB16" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>35438</v>
       </c>
       <c r="AC16" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>36878</v>
       </c>
       <c r="AD16" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>40338</v>
       </c>
       <c r="AE16" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>43556</v>
       </c>
       <c r="AF16" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>36087</v>
       </c>
       <c r="AG16" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>42380</v>
       </c>
       <c r="AH16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>51221.962080524681</v>
       </c>
       <c r="AI16" s="5">
-        <f>+AH16*(1+AI35)</f>
+        <f t="shared" ref="AI16:AQ16" si="11">+AH16*(1+AI35)</f>
         <v>53783.060184550915</v>
       </c>
       <c r="AJ16" s="5">
-        <f t="shared" ref="AJ16:AQ16" si="14">+AI16*(1+AJ35)</f>
+        <f t="shared" si="11"/>
         <v>56472.213193778465</v>
       </c>
       <c r="AK16" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>59295.823853467387</v>
       </c>
       <c r="AL16" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>62260.61504614076</v>
       </c>
       <c r="AM16" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>65373.645798447804</v>
       </c>
       <c r="AN16" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>68642.328088370195</v>
       </c>
       <c r="AO16" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>72074.444492788709</v>
       </c>
       <c r="AP16" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>75678.166717428147</v>
       </c>
       <c r="AQ16" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>79462.075053299559</v>
       </c>
     </row>
@@ -3639,43 +3841,43 @@
         <v>-73</v>
       </c>
       <c r="AH17" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>535.36528056112229</v>
       </c>
       <c r="AI17" s="3">
-        <f t="shared" ref="AI17:AQ17" si="15">+AI16*(AH17/AH16)</f>
+        <f t="shared" ref="AI17:AQ17" si="12">+AI16*(AH17/AH16)</f>
         <v>562.13354458917843</v>
       </c>
       <c r="AJ17" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>590.24022181863734</v>
       </c>
       <c r="AK17" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>619.75223290956922</v>
       </c>
       <c r="AL17" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>650.73984455504774</v>
       </c>
       <c r="AM17" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>683.27683678280016</v>
       </c>
       <c r="AN17" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>717.44067862194015</v>
       </c>
       <c r="AO17" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>753.31271255303727</v>
       </c>
       <c r="AP17" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>790.97834818068907</v>
       </c>
       <c r="AQ17" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>830.52726558972358</v>
       </c>
     </row>
@@ -3745,7 +3947,7 @@
         <v>596</v>
       </c>
       <c r="V18" s="3">
-        <f t="shared" ref="V18:V19" si="16">+V$16*(U18/U$16)</f>
+        <f>+V$16*(U18/U$16)</f>
         <v>550.36186190562944</v>
       </c>
       <c r="Z18" s="3">
@@ -3773,43 +3975,43 @@
         <v>-1155</v>
       </c>
       <c r="AH18" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1307.3618619056294</v>
       </c>
       <c r="AI18" s="3">
-        <f t="shared" ref="AI18:AQ18" si="17">+AI16*(AH18/AH16)</f>
+        <f t="shared" ref="AI18:AQ18" si="13">+AI16*(AH18/AH16)</f>
         <v>1372.7299550009109</v>
       </c>
       <c r="AJ18" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>1441.3664527509566</v>
       </c>
       <c r="AK18" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>1513.4347753885042</v>
       </c>
       <c r="AL18" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>1589.1065141579295</v>
       </c>
       <c r="AM18" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>1668.561839865826</v>
       </c>
       <c r="AN18" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>1751.9899318591174</v>
       </c>
       <c r="AO18" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>1839.5894284520734</v>
       </c>
       <c r="AP18" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>1931.5688998746771</v>
       </c>
       <c r="AQ18" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="13"/>
         <v>2028.147344868411</v>
       </c>
     </row>
@@ -3879,7 +4081,7 @@
         <v>17</v>
       </c>
       <c r="V19" s="3">
-        <f t="shared" si="16"/>
+        <f>+V$16*(U19/U$16)</f>
         <v>15.698241027509564</v>
       </c>
       <c r="Z19" s="3">
@@ -3907,43 +4109,43 @@
         <v>-191</v>
       </c>
       <c r="AH19" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>30.698241027509564</v>
       </c>
       <c r="AI19" s="3">
-        <f t="shared" ref="AI19:AQ19" si="18">+AI16*(AH19/AH16)</f>
+        <f t="shared" ref="AI19:AQ19" si="14">+AI16*(AH19/AH16)</f>
         <v>32.233153078885046</v>
       </c>
       <c r="AJ19" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>33.844810732829302</v>
       </c>
       <c r="AK19" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>35.537051269470766</v>
       </c>
       <c r="AL19" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>37.313903832944305</v>
       </c>
       <c r="AM19" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>39.179599024591525</v>
       </c>
       <c r="AN19" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>41.138578975821105</v>
       </c>
       <c r="AO19" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>43.195507924612158</v>
       </c>
       <c r="AP19" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>45.355283320842773</v>
       </c>
       <c r="AQ19" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="14"/>
         <v>47.623047486884914</v>
       </c>
     </row>
@@ -4033,75 +4235,75 @@
       </c>
       <c r="X20" s="17"/>
       <c r="Z20" s="3">
-        <f t="shared" ref="Z20:AG20" si="19">+SUM(Z17:Z19)</f>
+        <f t="shared" ref="Z20:AG20" si="15">+SUM(Z17:Z19)</f>
         <v>2044</v>
       </c>
       <c r="AA20" s="16">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>1988</v>
       </c>
       <c r="AB20" s="16">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>2027</v>
       </c>
       <c r="AC20" s="16">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>2760</v>
       </c>
       <c r="AD20" s="16">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>3352</v>
       </c>
       <c r="AE20" s="16">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>3573</v>
       </c>
       <c r="AF20" s="16">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>4730</v>
       </c>
       <c r="AG20" s="16">
-        <f t="shared" si="19"/>
+        <f t="shared" si="15"/>
         <v>-1419</v>
       </c>
       <c r="AH20" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1873.4253834942613</v>
       </c>
       <c r="AI20" s="16">
-        <f t="shared" ref="AI20:AQ20" si="20">+SUM(AI17:AI19)</f>
+        <f t="shared" ref="AI20:AQ20" si="16">+SUM(AI17:AI19)</f>
         <v>1967.0966526689745</v>
       </c>
       <c r="AJ20" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>2065.4514853024234</v>
       </c>
       <c r="AK20" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>2168.7240595675444</v>
       </c>
       <c r="AL20" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>2277.1602625459213</v>
       </c>
       <c r="AM20" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>2391.0182756732174</v>
       </c>
       <c r="AN20" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>2510.5691894568786</v>
       </c>
       <c r="AO20" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>2636.0976489297232</v>
       </c>
       <c r="AP20" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>2767.902531376209</v>
       </c>
       <c r="AQ20" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="16"/>
         <v>2906.2976579450192</v>
       </c>
     </row>
@@ -4191,75 +4393,75 @@
       </c>
       <c r="X21" s="13"/>
       <c r="Z21" s="5">
-        <f t="shared" ref="Z21:AG21" si="21">+Z16-Z20</f>
+        <f t="shared" ref="Z21:AG21" si="17">+Z16-Z20</f>
         <v>32144</v>
       </c>
       <c r="AA21" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>30830</v>
       </c>
       <c r="AB21" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>33411</v>
       </c>
       <c r="AC21" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>34118</v>
       </c>
       <c r="AD21" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>36986</v>
       </c>
       <c r="AE21" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>39983</v>
       </c>
       <c r="AF21" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>31357</v>
       </c>
       <c r="AG21" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="17"/>
         <v>43799</v>
       </c>
       <c r="AH21" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>49348.536697030424</v>
       </c>
       <c r="AI21" s="5">
-        <f t="shared" ref="AI21:AQ21" si="22">+AI16-AI20</f>
+        <f t="shared" ref="AI21:AQ21" si="18">+AI16-AI20</f>
         <v>51815.963531881942</v>
       </c>
       <c r="AJ21" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>54406.761708476042</v>
       </c>
       <c r="AK21" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>57127.099793899841</v>
       </c>
       <c r="AL21" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>59983.45478359484</v>
       </c>
       <c r="AM21" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>62982.627522774586</v>
       </c>
       <c r="AN21" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>66131.758898913322</v>
       </c>
       <c r="AO21" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>69438.346843858992</v>
       </c>
       <c r="AP21" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>72910.264186051936</v>
       </c>
       <c r="AQ21" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="18"/>
         <v>76555.77739535454</v>
       </c>
     </row>
@@ -4360,43 +4562,43 @@
         <v>9053</v>
       </c>
       <c r="AH22" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10273.925600291492</v>
       </c>
       <c r="AI22" s="3">
-        <f t="shared" ref="AI22:AQ22" si="23">+AI21*(AH22/AH21)</f>
+        <f t="shared" ref="AI22:AQ22" si="19">+AI21*(AH22/AH21)</f>
         <v>10787.621880306066</v>
       </c>
       <c r="AJ22" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>11327.002974321369</v>
       </c>
       <c r="AK22" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>11893.353123037437</v>
       </c>
       <c r="AL22" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>12488.02077918931</v>
       </c>
       <c r="AM22" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>13112.421818148776</v>
       </c>
       <c r="AN22" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>13768.042909056216</v>
       </c>
       <c r="AO22" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>14456.445054509026</v>
       </c>
       <c r="AP22" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>15179.267307234477</v>
       </c>
       <c r="AQ22" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="19"/>
         <v>15938.230672596203</v>
       </c>
     </row>
@@ -4466,7 +4668,7 @@
         <v>3571</v>
       </c>
       <c r="V23" s="3">
-        <f t="shared" ref="V23:V26" si="24">+V$21*(U23/U$21)</f>
+        <f>+V$21*(U23/U$21)</f>
         <v>3297.5540417198031</v>
       </c>
       <c r="Z23" s="3">
@@ -4494,43 +4696,43 @@
         <v>11007</v>
       </c>
       <c r="AH23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>13570.554041719803</v>
       </c>
       <c r="AI23" s="3">
-        <f t="shared" ref="AI23:AQ23" si="25">+AI21*(AH23/AH21)</f>
+        <f t="shared" ref="AI23:AQ23" si="20">+AI21*(AH23/AH21)</f>
         <v>14249.081743805791</v>
       </c>
       <c r="AJ23" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>14961.535830996081</v>
       </c>
       <c r="AK23" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>15709.612622545885</v>
       </c>
       <c r="AL23" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>16495.093253673182</v>
       </c>
       <c r="AM23" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>17319.847916356841</v>
       </c>
       <c r="AN23" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>18185.840312174685</v>
       </c>
       <c r="AO23" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>19095.13232778342</v>
       </c>
       <c r="AP23" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>20049.888944172588</v>
       </c>
       <c r="AQ23" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="20"/>
         <v>21052.38339138122</v>
       </c>
     </row>
@@ -4600,7 +4802,7 @@
         <v>774</v>
       </c>
       <c r="V24" s="3">
-        <f t="shared" si="24"/>
+        <f>+V$21*(U24/U$21)</f>
         <v>714.73167972308249</v>
       </c>
       <c r="Z24" s="3">
@@ -4628,43 +4830,43 @@
         <v>1993</v>
       </c>
       <c r="AH24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2792.7316797230824</v>
       </c>
       <c r="AI24" s="3">
-        <f t="shared" ref="AI24:AQ24" si="26">+AI21*(AH24/AH21)</f>
+        <f t="shared" ref="AI24:AQ24" si="21">+AI21*(AH24/AH21)</f>
         <v>2932.3682637092365</v>
       </c>
       <c r="AJ24" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>3078.9866768946986</v>
       </c>
       <c r="AK24" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>3232.9360107394332</v>
       </c>
       <c r="AL24" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>3394.5828112764052</v>
       </c>
       <c r="AM24" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>3564.3119518402259</v>
       </c>
       <c r="AN24" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>3742.5275494322373</v>
       </c>
       <c r="AO24" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>3929.6539269038494</v>
       </c>
       <c r="AP24" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>4126.1366232490418</v>
       </c>
       <c r="AQ24" s="3">
-        <f t="shared" si="26"/>
+        <f t="shared" si="21"/>
         <v>4332.4434544114938</v>
       </c>
     </row>
@@ -4734,7 +4936,7 @@
         <v>1748</v>
       </c>
       <c r="V25" s="3">
-        <f t="shared" si="24"/>
+        <f>+V$21*(U25/U$21)</f>
         <v>1614.1485480051012</v>
       </c>
       <c r="Z25" s="3">
@@ -4762,43 +4964,43 @@
         <v>6240</v>
       </c>
       <c r="AH25" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>6832.1485480051015</v>
       </c>
       <c r="AI25" s="3">
-        <f t="shared" ref="AI25:AQ25" si="27">+AI21*(AH25/AH21)</f>
+        <f t="shared" ref="AI25:AQ25" si="22">+AI21*(AH25/AH21)</f>
         <v>7173.7559754053564</v>
       </c>
       <c r="AJ25" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="22"/>
         <v>7532.4437741756246</v>
       </c>
       <c r="AK25" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="22"/>
         <v>7909.0659628844051</v>
       </c>
       <c r="AL25" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="22"/>
         <v>8304.5192610286267</v>
       </c>
       <c r="AM25" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="22"/>
         <v>8719.7452240800576</v>
       </c>
       <c r="AN25" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="22"/>
         <v>9155.7324852840611</v>
       </c>
       <c r="AO25" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="22"/>
         <v>9613.519109548266</v>
       </c>
       <c r="AP25" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="22"/>
         <v>10094.195065025679</v>
       </c>
       <c r="AQ25" s="3">
-        <f t="shared" si="27"/>
+        <f t="shared" si="22"/>
         <v>10598.904818276962</v>
       </c>
     </row>
@@ -4868,7 +5070,7 @@
         <v>1574</v>
       </c>
       <c r="V26" s="3">
-        <f t="shared" si="24"/>
+        <f>+V$21*(U26/U$21)</f>
         <v>1453.4724339588267</v>
       </c>
       <c r="Z26" s="3">
@@ -4896,43 +5098,43 @@
         <v>4817</v>
       </c>
       <c r="AH26" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>5876.4724339588265</v>
       </c>
       <c r="AI26" s="3">
-        <f t="shared" ref="AI26:AQ26" si="28">+AI21*(AH26/AH21)</f>
+        <f t="shared" ref="AI26:AQ26" si="23">+AI21*(AH26/AH21)</f>
         <v>6170.2960556567677</v>
       </c>
       <c r="AJ26" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="23"/>
         <v>6478.8108584396059</v>
       </c>
       <c r="AK26" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="23"/>
         <v>6802.7514013615864</v>
       </c>
       <c r="AL26" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="23"/>
         <v>7142.8889714296674</v>
       </c>
       <c r="AM26" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="23"/>
         <v>7500.0334200011521</v>
       </c>
       <c r="AN26" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="23"/>
         <v>7875.0350910012103</v>
       </c>
       <c r="AO26" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="23"/>
         <v>8268.7868455512707</v>
       </c>
       <c r="AP26" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="23"/>
         <v>8682.2261878288336</v>
       </c>
       <c r="AQ26" s="3">
-        <f t="shared" si="28"/>
+        <f t="shared" si="23"/>
         <v>9116.3374972202764</v>
       </c>
     </row>
@@ -5021,75 +5223,75 @@
         <v>9528.8323036983056</v>
       </c>
       <c r="Z27" s="3">
-        <f t="shared" ref="Z27:AG27" si="29">+SUM(Z22:Z26)</f>
+        <f t="shared" ref="Z27:AG27" si="24">+SUM(Z22:Z26)</f>
         <v>23153</v>
       </c>
       <c r="AA27" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="24"/>
         <v>22892</v>
       </c>
       <c r="AB27" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="24"/>
         <v>25369</v>
       </c>
       <c r="AC27" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="24"/>
         <v>26693</v>
       </c>
       <c r="AD27" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="24"/>
         <v>28864</v>
       </c>
       <c r="AE27" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="24"/>
         <v>31554</v>
       </c>
       <c r="AF27" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="24"/>
         <v>27061</v>
       </c>
       <c r="AG27" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="24"/>
         <v>33110</v>
       </c>
       <c r="AH27" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>39345.832303698306</v>
       </c>
       <c r="AI27" s="3">
-        <f t="shared" ref="AI27:AQ27" si="30">+SUM(AI22:AI26)</f>
+        <f t="shared" ref="AI27:AQ27" si="25">+SUM(AI22:AI26)</f>
         <v>41313.123918883219</v>
       </c>
       <c r="AJ27" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="25"/>
         <v>43378.780114827379</v>
       </c>
       <c r="AK27" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="25"/>
         <v>45547.719120568749</v>
       </c>
       <c r="AL27" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="25"/>
         <v>47825.105076597189</v>
       </c>
       <c r="AM27" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="25"/>
         <v>50216.360330427044</v>
       </c>
       <c r="AN27" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="25"/>
         <v>52727.178346948407</v>
       </c>
       <c r="AO27" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="25"/>
         <v>55363.537264295832</v>
       </c>
       <c r="AP27" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="25"/>
         <v>58131.714127510619</v>
       </c>
       <c r="AQ27" s="3">
-        <f t="shared" si="30"/>
+        <f t="shared" si="25"/>
         <v>61038.299833886151</v>
       </c>
     </row>
@@ -5179,75 +5381,75 @@
       </c>
       <c r="X28" s="13"/>
       <c r="Z28" s="5">
-        <f t="shared" ref="Z28:AG28" si="31">+Z21-Z27</f>
+        <f t="shared" ref="Z28:AG28" si="26">+Z21-Z27</f>
         <v>8991</v>
       </c>
       <c r="AA28" s="5">
-        <f t="shared" si="31"/>
+        <f t="shared" si="26"/>
         <v>7938</v>
       </c>
       <c r="AB28" s="5">
-        <f t="shared" si="31"/>
+        <f t="shared" si="26"/>
         <v>8042</v>
       </c>
       <c r="AC28" s="5">
-        <f t="shared" si="31"/>
+        <f t="shared" si="26"/>
         <v>7425</v>
       </c>
       <c r="AD28" s="5">
-        <f t="shared" si="31"/>
+        <f t="shared" si="26"/>
         <v>8122</v>
       </c>
       <c r="AE28" s="5">
-        <f t="shared" si="31"/>
+        <f t="shared" si="26"/>
         <v>8429</v>
       </c>
       <c r="AF28" s="5">
-        <f t="shared" si="31"/>
+        <f t="shared" si="26"/>
         <v>4296</v>
       </c>
       <c r="AG28" s="5">
-        <f t="shared" si="31"/>
+        <f t="shared" si="26"/>
         <v>10689</v>
       </c>
       <c r="AH28" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10002.704393332118</v>
       </c>
       <c r="AI28" s="5">
-        <f t="shared" ref="AI28:AQ28" si="32">+AI21-AI27</f>
+        <f t="shared" ref="AI28:AQ28" si="27">+AI21-AI27</f>
         <v>10502.839612998723</v>
       </c>
       <c r="AJ28" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>11027.981593648663</v>
       </c>
       <c r="AK28" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>11579.380673331092</v>
       </c>
       <c r="AL28" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>12158.349706997651</v>
       </c>
       <c r="AM28" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>12766.267192347543</v>
       </c>
       <c r="AN28" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>13404.580551964915</v>
       </c>
       <c r="AO28" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>14074.80957956316</v>
       </c>
       <c r="AP28" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>14778.550058541317</v>
       </c>
       <c r="AQ28" s="5">
-        <f t="shared" si="32"/>
+        <f t="shared" si="27"/>
         <v>15517.477561468389</v>
       </c>
     </row>
@@ -5345,7 +5547,7 @@
         <v>2629</v>
       </c>
       <c r="AH29" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2273.5870468209146</v>
       </c>
       <c r="AI29" s="3">
@@ -5353,35 +5555,35 @@
         <v>2625.7099032496808</v>
       </c>
       <c r="AJ29" s="3">
-        <f t="shared" ref="AJ29:AQ29" si="33">+AJ28*0.25</f>
+        <f t="shared" ref="AJ29:AQ29" si="28">+AJ28*0.25</f>
         <v>2756.9953984121657</v>
       </c>
       <c r="AK29" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>2894.845168332773</v>
       </c>
       <c r="AL29" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>3039.5874267494128</v>
       </c>
       <c r="AM29" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>3191.5667980868857</v>
       </c>
       <c r="AN29" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>3351.1451379912287</v>
       </c>
       <c r="AO29" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>3518.7023948907899</v>
       </c>
       <c r="AP29" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>3694.6375146353294</v>
       </c>
       <c r="AQ29" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="28"/>
         <v>3879.3693903670974</v>
       </c>
     </row>
@@ -5471,511 +5673,511 @@
       </c>
       <c r="X30" s="13"/>
       <c r="Z30" s="5">
-        <f t="shared" ref="Z30:AI30" si="34">+Z28-Z29</f>
+        <f t="shared" ref="Z30:AI30" si="29">+Z28-Z29</f>
         <v>5885</v>
       </c>
       <c r="AA30" s="5">
+        <f t="shared" si="29"/>
+        <v>5163</v>
+      </c>
+      <c r="AB30" s="5">
+        <f t="shared" si="29"/>
+        <v>5375</v>
+      </c>
+      <c r="AC30" s="5">
+        <f t="shared" si="29"/>
+        <v>2748</v>
+      </c>
+      <c r="AD30" s="5">
+        <f t="shared" si="29"/>
+        <v>6921</v>
+      </c>
+      <c r="AE30" s="5">
+        <f t="shared" si="29"/>
+        <v>6759</v>
+      </c>
+      <c r="AF30" s="5">
+        <f t="shared" si="29"/>
+        <v>3135</v>
+      </c>
+      <c r="AG30" s="5">
+        <f t="shared" si="29"/>
+        <v>8060</v>
+      </c>
+      <c r="AH30" s="3">
+        <f t="shared" si="5"/>
+        <v>7729.1173465112042</v>
+      </c>
+      <c r="AI30" s="5">
+        <f t="shared" si="29"/>
+        <v>7877.1297097490424</v>
+      </c>
+      <c r="AJ30" s="5">
+        <f t="shared" ref="AJ30:AQ30" si="30">+AJ28-AJ29</f>
+        <v>8270.9861952364972</v>
+      </c>
+      <c r="AK30" s="5">
+        <f t="shared" si="30"/>
+        <v>8684.5355049983191</v>
+      </c>
+      <c r="AL30" s="5">
+        <f t="shared" si="30"/>
+        <v>9118.7622802482383</v>
+      </c>
+      <c r="AM30" s="5">
+        <f t="shared" si="30"/>
+        <v>9574.700394260657</v>
+      </c>
+      <c r="AN30" s="5">
+        <f t="shared" si="30"/>
+        <v>10053.435413973686</v>
+      </c>
+      <c r="AO30" s="5">
+        <f t="shared" si="30"/>
+        <v>10556.10718467237</v>
+      </c>
+      <c r="AP30" s="5">
+        <f t="shared" si="30"/>
+        <v>11083.912543905988</v>
+      </c>
+      <c r="AQ30" s="5">
+        <f t="shared" si="30"/>
+        <v>11638.108171101292</v>
+      </c>
+      <c r="AR30" s="5">
+        <f t="shared" ref="AR30:BW30" si="31">+AQ30*(1+$AU$36)</f>
+        <v>11754.489252812305</v>
+      </c>
+      <c r="AS30" s="5">
+        <f t="shared" si="31"/>
+        <v>11872.034145340429</v>
+      </c>
+      <c r="AT30" s="5">
+        <f t="shared" si="31"/>
+        <v>11990.754486793834</v>
+      </c>
+      <c r="AU30" s="5">
+        <f t="shared" si="31"/>
+        <v>12110.662031661772</v>
+      </c>
+      <c r="AV30" s="5">
+        <f t="shared" si="31"/>
+        <v>12231.768651978389</v>
+      </c>
+      <c r="AW30" s="5">
+        <f t="shared" si="31"/>
+        <v>12354.086338498173</v>
+      </c>
+      <c r="AX30" s="5">
+        <f t="shared" si="31"/>
+        <v>12477.627201883155</v>
+      </c>
+      <c r="AY30" s="5">
+        <f t="shared" si="31"/>
+        <v>12602.403473901986</v>
+      </c>
+      <c r="AZ30" s="5">
+        <f t="shared" si="31"/>
+        <v>12728.427508641007</v>
+      </c>
+      <c r="BA30" s="5">
+        <f t="shared" si="31"/>
+        <v>12855.711783727418</v>
+      </c>
+      <c r="BB30" s="5">
+        <f t="shared" si="31"/>
+        <v>12984.268901564692</v>
+      </c>
+      <c r="BC30" s="5">
+        <f t="shared" si="31"/>
+        <v>13114.11159058034</v>
+      </c>
+      <c r="BD30" s="5">
+        <f t="shared" si="31"/>
+        <v>13245.252706486144</v>
+      </c>
+      <c r="BE30" s="5">
+        <f t="shared" si="31"/>
+        <v>13377.705233551005</v>
+      </c>
+      <c r="BF30" s="5">
+        <f t="shared" si="31"/>
+        <v>13511.482285886515</v>
+      </c>
+      <c r="BG30" s="5">
+        <f t="shared" si="31"/>
+        <v>13646.59710874538</v>
+      </c>
+      <c r="BH30" s="5">
+        <f t="shared" si="31"/>
+        <v>13783.063079832835</v>
+      </c>
+      <c r="BI30" s="5">
+        <f t="shared" si="31"/>
+        <v>13920.893710631164</v>
+      </c>
+      <c r="BJ30" s="5">
+        <f t="shared" si="31"/>
+        <v>14060.102647737476</v>
+      </c>
+      <c r="BK30" s="5">
+        <f t="shared" si="31"/>
+        <v>14200.70367421485</v>
+      </c>
+      <c r="BL30" s="5">
+        <f t="shared" si="31"/>
+        <v>14342.710710956999</v>
+      </c>
+      <c r="BM30" s="5">
+        <f t="shared" si="31"/>
+        <v>14486.137818066569</v>
+      </c>
+      <c r="BN30" s="5">
+        <f t="shared" si="31"/>
+        <v>14630.999196247234</v>
+      </c>
+      <c r="BO30" s="5">
+        <f t="shared" si="31"/>
+        <v>14777.309188209707</v>
+      </c>
+      <c r="BP30" s="5">
+        <f t="shared" si="31"/>
+        <v>14925.082280091805</v>
+      </c>
+      <c r="BQ30" s="5">
+        <f t="shared" si="31"/>
+        <v>15074.333102892722</v>
+      </c>
+      <c r="BR30" s="5">
+        <f t="shared" si="31"/>
+        <v>15225.076433921649</v>
+      </c>
+      <c r="BS30" s="5">
+        <f t="shared" si="31"/>
+        <v>15377.327198260866</v>
+      </c>
+      <c r="BT30" s="5">
+        <f t="shared" si="31"/>
+        <v>15531.100470243475</v>
+      </c>
+      <c r="BU30" s="5">
+        <f t="shared" si="31"/>
+        <v>15686.41147494591</v>
+      </c>
+      <c r="BV30" s="5">
+        <f t="shared" si="31"/>
+        <v>15843.275589695369</v>
+      </c>
+      <c r="BW30" s="5">
+        <f t="shared" si="31"/>
+        <v>16001.708345592324</v>
+      </c>
+      <c r="BX30" s="5">
+        <f t="shared" ref="BX30:DC30" si="32">+BW30*(1+$AU$36)</f>
+        <v>16161.725429048247</v>
+      </c>
+      <c r="BY30" s="5">
+        <f t="shared" si="32"/>
+        <v>16323.342683338729</v>
+      </c>
+      <c r="BZ30" s="5">
+        <f t="shared" si="32"/>
+        <v>16486.576110172118</v>
+      </c>
+      <c r="CA30" s="5">
+        <f t="shared" si="32"/>
+        <v>16651.441871273841</v>
+      </c>
+      <c r="CB30" s="5">
+        <f t="shared" si="32"/>
+        <v>16817.956289986578</v>
+      </c>
+      <c r="CC30" s="5">
+        <f t="shared" si="32"/>
+        <v>16986.135852886444</v>
+      </c>
+      <c r="CD30" s="5">
+        <f t="shared" si="32"/>
+        <v>17155.99721141531</v>
+      </c>
+      <c r="CE30" s="5">
+        <f t="shared" si="32"/>
+        <v>17327.557183529461</v>
+      </c>
+      <c r="CF30" s="5">
+        <f t="shared" si="32"/>
+        <v>17500.832755364758</v>
+      </c>
+      <c r="CG30" s="5">
+        <f t="shared" si="32"/>
+        <v>17675.841082918407</v>
+      </c>
+      <c r="CH30" s="5">
+        <f t="shared" si="32"/>
+        <v>17852.599493747592</v>
+      </c>
+      <c r="CI30" s="5">
+        <f t="shared" si="32"/>
+        <v>18031.125488685069</v>
+      </c>
+      <c r="CJ30" s="5">
+        <f t="shared" si="32"/>
+        <v>18211.436743571921</v>
+      </c>
+      <c r="CK30" s="5">
+        <f t="shared" si="32"/>
+        <v>18393.55111100764</v>
+      </c>
+      <c r="CL30" s="5">
+        <f t="shared" si="32"/>
+        <v>18577.486622117718</v>
+      </c>
+      <c r="CM30" s="5">
+        <f t="shared" si="32"/>
+        <v>18763.261488338896</v>
+      </c>
+      <c r="CN30" s="5">
+        <f t="shared" si="32"/>
+        <v>18950.894103222287</v>
+      </c>
+      <c r="CO30" s="5">
+        <f t="shared" si="32"/>
+        <v>19140.403044254508</v>
+      </c>
+      <c r="CP30" s="5">
+        <f t="shared" si="32"/>
+        <v>19331.807074697052</v>
+      </c>
+      <c r="CQ30" s="5">
+        <f t="shared" si="32"/>
+        <v>19525.125145444021</v>
+      </c>
+      <c r="CR30" s="5">
+        <f t="shared" si="32"/>
+        <v>19720.37639689846</v>
+      </c>
+      <c r="CS30" s="5">
+        <f t="shared" si="32"/>
+        <v>19917.580160867445</v>
+      </c>
+      <c r="CT30" s="5">
+        <f t="shared" si="32"/>
+        <v>20116.75596247612</v>
+      </c>
+      <c r="CU30" s="5">
+        <f t="shared" si="32"/>
+        <v>20317.923522100882</v>
+      </c>
+      <c r="CV30" s="5">
+        <f t="shared" si="32"/>
+        <v>20521.102757321893</v>
+      </c>
+      <c r="CW30" s="5">
+        <f t="shared" si="32"/>
+        <v>20726.313784895112</v>
+      </c>
+      <c r="CX30" s="5">
+        <f t="shared" si="32"/>
+        <v>20933.576922744061</v>
+      </c>
+      <c r="CY30" s="5">
+        <f t="shared" si="32"/>
+        <v>21142.912691971502</v>
+      </c>
+      <c r="CZ30" s="5">
+        <f t="shared" si="32"/>
+        <v>21354.341818891218</v>
+      </c>
+      <c r="DA30" s="5">
+        <f t="shared" si="32"/>
+        <v>21567.885237080132</v>
+      </c>
+      <c r="DB30" s="5">
+        <f t="shared" si="32"/>
+        <v>21783.564089450934</v>
+      </c>
+      <c r="DC30" s="5">
+        <f t="shared" si="32"/>
+        <v>22001.399730345445</v>
+      </c>
+      <c r="DD30" s="5">
+        <f t="shared" ref="DD30:EI30" si="33">+DC30*(1+$AU$36)</f>
+        <v>22221.413727648898</v>
+      </c>
+      <c r="DE30" s="5">
+        <f t="shared" si="33"/>
+        <v>22443.627864925387</v>
+      </c>
+      <c r="DF30" s="5">
+        <f t="shared" si="33"/>
+        <v>22668.06414357464</v>
+      </c>
+      <c r="DG30" s="5">
+        <f t="shared" si="33"/>
+        <v>22894.744785010385</v>
+      </c>
+      <c r="DH30" s="5">
+        <f t="shared" si="33"/>
+        <v>23123.692232860489</v>
+      </c>
+      <c r="DI30" s="5">
+        <f t="shared" si="33"/>
+        <v>23354.929155189093</v>
+      </c>
+      <c r="DJ30" s="5">
+        <f t="shared" si="33"/>
+        <v>23588.478446740985</v>
+      </c>
+      <c r="DK30" s="5">
+        <f t="shared" si="33"/>
+        <v>23824.363231208394</v>
+      </c>
+      <c r="DL30" s="5">
+        <f t="shared" si="33"/>
+        <v>24062.606863520479</v>
+      </c>
+      <c r="DM30" s="5">
+        <f t="shared" si="33"/>
+        <v>24303.232932155683</v>
+      </c>
+      <c r="DN30" s="5">
+        <f t="shared" si="33"/>
+        <v>24546.265261477241</v>
+      </c>
+      <c r="DO30" s="5">
+        <f t="shared" si="33"/>
+        <v>24791.727914092015</v>
+      </c>
+      <c r="DP30" s="5">
+        <f t="shared" si="33"/>
+        <v>25039.645193232936</v>
+      </c>
+      <c r="DQ30" s="5">
+        <f t="shared" si="33"/>
+        <v>25290.041645165267</v>
+      </c>
+      <c r="DR30" s="5">
+        <f t="shared" si="33"/>
+        <v>25542.942061616919</v>
+      </c>
+      <c r="DS30" s="5">
+        <f t="shared" si="33"/>
+        <v>25798.371482233088</v>
+      </c>
+      <c r="DT30" s="5">
+        <f t="shared" si="33"/>
+        <v>26056.355197055418</v>
+      </c>
+      <c r="DU30" s="5">
+        <f t="shared" si="33"/>
+        <v>26316.918749025972</v>
+      </c>
+      <c r="DV30" s="5">
+        <f t="shared" si="33"/>
+        <v>26580.087936516233</v>
+      </c>
+      <c r="DW30" s="5">
+        <f t="shared" si="33"/>
+        <v>26845.888815881397</v>
+      </c>
+      <c r="DX30" s="5">
+        <f t="shared" si="33"/>
+        <v>27114.34770404021</v>
+      </c>
+      <c r="DY30" s="5">
+        <f t="shared" si="33"/>
+        <v>27385.491181080612</v>
+      </c>
+      <c r="DZ30" s="5">
+        <f t="shared" si="33"/>
+        <v>27659.346092891417</v>
+      </c>
+      <c r="EA30" s="5">
+        <f t="shared" si="33"/>
+        <v>27935.939553820332</v>
+      </c>
+      <c r="EB30" s="5">
+        <f t="shared" si="33"/>
+        <v>28215.298949358534</v>
+      </c>
+      <c r="EC30" s="5">
+        <f t="shared" si="33"/>
+        <v>28497.451938852118</v>
+      </c>
+      <c r="ED30" s="5">
+        <f t="shared" si="33"/>
+        <v>28782.426458240639</v>
+      </c>
+      <c r="EE30" s="5">
+        <f t="shared" si="33"/>
+        <v>29070.250722823046</v>
+      </c>
+      <c r="EF30" s="5">
+        <f t="shared" si="33"/>
+        <v>29360.953230051276</v>
+      </c>
+      <c r="EG30" s="5">
+        <f t="shared" si="33"/>
+        <v>29654.56276235179</v>
+      </c>
+      <c r="EH30" s="5">
+        <f t="shared" si="33"/>
+        <v>29951.10838997531</v>
+      </c>
+      <c r="EI30" s="5">
+        <f t="shared" si="33"/>
+        <v>30250.619473875064</v>
+      </c>
+      <c r="EJ30" s="5">
+        <f t="shared" ref="EJ30:EV30" si="34">+EI30*(1+$AU$36)</f>
+        <v>30553.125668613815</v>
+      </c>
+      <c r="EK30" s="5">
         <f t="shared" si="34"/>
-        <v>5163</v>
-      </c>
-      <c r="AB30" s="5">
+        <v>30858.656925299954</v>
+      </c>
+      <c r="EL30" s="5">
         <f t="shared" si="34"/>
-        <v>5375</v>
-      </c>
-      <c r="AC30" s="5">
+        <v>31167.243494552953</v>
+      </c>
+      <c r="EM30" s="5">
         <f t="shared" si="34"/>
-        <v>2748</v>
-      </c>
-      <c r="AD30" s="5">
+        <v>31478.915929498482</v>
+      </c>
+      <c r="EN30" s="5">
         <f t="shared" si="34"/>
-        <v>6921</v>
-      </c>
-      <c r="AE30" s="5">
+        <v>31793.705088793467</v>
+      </c>
+      <c r="EO30" s="5">
         <f t="shared" si="34"/>
-        <v>6759</v>
-      </c>
-      <c r="AF30" s="5">
+        <v>32111.642139681404</v>
+      </c>
+      <c r="EP30" s="5">
         <f t="shared" si="34"/>
-        <v>3135</v>
-      </c>
-      <c r="AG30" s="5">
+        <v>32432.758561078219</v>
+      </c>
+      <c r="EQ30" s="5">
         <f t="shared" si="34"/>
-        <v>8060</v>
-      </c>
-      <c r="AH30" s="3">
-        <f t="shared" si="6"/>
-        <v>7729.1173465112042</v>
-      </c>
-      <c r="AI30" s="5">
+        <v>32757.086146689002</v>
+      </c>
+      <c r="ER30" s="5">
         <f t="shared" si="34"/>
-        <v>7877.1297097490424</v>
-      </c>
-      <c r="AJ30" s="5">
-        <f t="shared" ref="AJ30:AQ30" si="35">+AJ28-AJ29</f>
-        <v>8270.9861952364972</v>
-      </c>
-      <c r="AK30" s="5">
-        <f t="shared" si="35"/>
-        <v>8684.5355049983191</v>
-      </c>
-      <c r="AL30" s="5">
-        <f t="shared" si="35"/>
-        <v>9118.7622802482383</v>
-      </c>
-      <c r="AM30" s="5">
-        <f t="shared" si="35"/>
-        <v>9574.700394260657</v>
-      </c>
-      <c r="AN30" s="5">
-        <f t="shared" si="35"/>
-        <v>10053.435413973686</v>
-      </c>
-      <c r="AO30" s="5">
-        <f t="shared" si="35"/>
-        <v>10556.10718467237</v>
-      </c>
-      <c r="AP30" s="5">
-        <f t="shared" si="35"/>
-        <v>11083.912543905988</v>
-      </c>
-      <c r="AQ30" s="5">
-        <f t="shared" si="35"/>
-        <v>11638.108171101292</v>
-      </c>
-      <c r="AR30" s="5">
-        <f>+AQ30*(1+$AU$36)</f>
-        <v>11754.489252812305</v>
-      </c>
-      <c r="AS30" s="5">
-        <f t="shared" ref="AS30:DD30" si="36">+AR30*(1+$AU$36)</f>
-        <v>11872.034145340429</v>
-      </c>
-      <c r="AT30" s="5">
-        <f t="shared" si="36"/>
-        <v>11990.754486793834</v>
-      </c>
-      <c r="AU30" s="5">
-        <f t="shared" si="36"/>
-        <v>12110.662031661772</v>
-      </c>
-      <c r="AV30" s="5">
-        <f t="shared" si="36"/>
-        <v>12231.768651978389</v>
-      </c>
-      <c r="AW30" s="5">
-        <f t="shared" si="36"/>
-        <v>12354.086338498173</v>
-      </c>
-      <c r="AX30" s="5">
-        <f t="shared" si="36"/>
-        <v>12477.627201883155</v>
-      </c>
-      <c r="AY30" s="5">
-        <f t="shared" si="36"/>
-        <v>12602.403473901986</v>
-      </c>
-      <c r="AZ30" s="5">
-        <f t="shared" si="36"/>
-        <v>12728.427508641007</v>
-      </c>
-      <c r="BA30" s="5">
-        <f t="shared" si="36"/>
-        <v>12855.711783727418</v>
-      </c>
-      <c r="BB30" s="5">
-        <f t="shared" si="36"/>
-        <v>12984.268901564692</v>
-      </c>
-      <c r="BC30" s="5">
-        <f t="shared" si="36"/>
-        <v>13114.11159058034</v>
-      </c>
-      <c r="BD30" s="5">
-        <f t="shared" si="36"/>
-        <v>13245.252706486144</v>
-      </c>
-      <c r="BE30" s="5">
-        <f t="shared" si="36"/>
-        <v>13377.705233551005</v>
-      </c>
-      <c r="BF30" s="5">
-        <f t="shared" si="36"/>
-        <v>13511.482285886515</v>
-      </c>
-      <c r="BG30" s="5">
-        <f t="shared" si="36"/>
-        <v>13646.59710874538</v>
-      </c>
-      <c r="BH30" s="5">
-        <f t="shared" si="36"/>
-        <v>13783.063079832835</v>
-      </c>
-      <c r="BI30" s="5">
-        <f t="shared" si="36"/>
-        <v>13920.893710631164</v>
-      </c>
-      <c r="BJ30" s="5">
-        <f t="shared" si="36"/>
-        <v>14060.102647737476</v>
-      </c>
-      <c r="BK30" s="5">
-        <f t="shared" si="36"/>
-        <v>14200.70367421485</v>
-      </c>
-      <c r="BL30" s="5">
-        <f t="shared" si="36"/>
-        <v>14342.710710956999</v>
-      </c>
-      <c r="BM30" s="5">
-        <f t="shared" si="36"/>
-        <v>14486.137818066569</v>
-      </c>
-      <c r="BN30" s="5">
-        <f t="shared" si="36"/>
-        <v>14630.999196247234</v>
-      </c>
-      <c r="BO30" s="5">
-        <f t="shared" si="36"/>
-        <v>14777.309188209707</v>
-      </c>
-      <c r="BP30" s="5">
-        <f t="shared" si="36"/>
-        <v>14925.082280091805</v>
-      </c>
-      <c r="BQ30" s="5">
-        <f t="shared" si="36"/>
-        <v>15074.333102892722</v>
-      </c>
-      <c r="BR30" s="5">
-        <f t="shared" si="36"/>
-        <v>15225.076433921649</v>
-      </c>
-      <c r="BS30" s="5">
-        <f t="shared" si="36"/>
-        <v>15377.327198260866</v>
-      </c>
-      <c r="BT30" s="5">
-        <f t="shared" si="36"/>
-        <v>15531.100470243475</v>
-      </c>
-      <c r="BU30" s="5">
-        <f t="shared" si="36"/>
-        <v>15686.41147494591</v>
-      </c>
-      <c r="BV30" s="5">
-        <f t="shared" si="36"/>
-        <v>15843.275589695369</v>
-      </c>
-      <c r="BW30" s="5">
-        <f t="shared" si="36"/>
-        <v>16001.708345592324</v>
-      </c>
-      <c r="BX30" s="5">
-        <f t="shared" si="36"/>
-        <v>16161.725429048247</v>
-      </c>
-      <c r="BY30" s="5">
-        <f t="shared" si="36"/>
-        <v>16323.342683338729</v>
-      </c>
-      <c r="BZ30" s="5">
-        <f t="shared" si="36"/>
-        <v>16486.576110172118</v>
-      </c>
-      <c r="CA30" s="5">
-        <f t="shared" si="36"/>
-        <v>16651.441871273841</v>
-      </c>
-      <c r="CB30" s="5">
-        <f t="shared" si="36"/>
-        <v>16817.956289986578</v>
-      </c>
-      <c r="CC30" s="5">
-        <f t="shared" si="36"/>
-        <v>16986.135852886444</v>
-      </c>
-      <c r="CD30" s="5">
-        <f t="shared" si="36"/>
-        <v>17155.99721141531</v>
-      </c>
-      <c r="CE30" s="5">
-        <f t="shared" si="36"/>
-        <v>17327.557183529461</v>
-      </c>
-      <c r="CF30" s="5">
-        <f t="shared" si="36"/>
-        <v>17500.832755364758</v>
-      </c>
-      <c r="CG30" s="5">
-        <f t="shared" si="36"/>
-        <v>17675.841082918407</v>
-      </c>
-      <c r="CH30" s="5">
-        <f t="shared" si="36"/>
-        <v>17852.599493747592</v>
-      </c>
-      <c r="CI30" s="5">
-        <f t="shared" si="36"/>
-        <v>18031.125488685069</v>
-      </c>
-      <c r="CJ30" s="5">
-        <f t="shared" si="36"/>
-        <v>18211.436743571921</v>
-      </c>
-      <c r="CK30" s="5">
-        <f t="shared" si="36"/>
-        <v>18393.55111100764</v>
-      </c>
-      <c r="CL30" s="5">
-        <f t="shared" si="36"/>
-        <v>18577.486622117718</v>
-      </c>
-      <c r="CM30" s="5">
-        <f t="shared" si="36"/>
-        <v>18763.261488338896</v>
-      </c>
-      <c r="CN30" s="5">
-        <f t="shared" si="36"/>
-        <v>18950.894103222287</v>
-      </c>
-      <c r="CO30" s="5">
-        <f t="shared" si="36"/>
-        <v>19140.403044254508</v>
-      </c>
-      <c r="CP30" s="5">
-        <f t="shared" si="36"/>
-        <v>19331.807074697052</v>
-      </c>
-      <c r="CQ30" s="5">
-        <f t="shared" si="36"/>
-        <v>19525.125145444021</v>
-      </c>
-      <c r="CR30" s="5">
-        <f t="shared" si="36"/>
-        <v>19720.37639689846</v>
-      </c>
-      <c r="CS30" s="5">
-        <f t="shared" si="36"/>
-        <v>19917.580160867445</v>
-      </c>
-      <c r="CT30" s="5">
-        <f t="shared" si="36"/>
-        <v>20116.75596247612</v>
-      </c>
-      <c r="CU30" s="5">
-        <f t="shared" si="36"/>
-        <v>20317.923522100882</v>
-      </c>
-      <c r="CV30" s="5">
-        <f t="shared" si="36"/>
-        <v>20521.102757321893</v>
-      </c>
-      <c r="CW30" s="5">
-        <f t="shared" si="36"/>
-        <v>20726.313784895112</v>
-      </c>
-      <c r="CX30" s="5">
-        <f t="shared" si="36"/>
-        <v>20933.576922744061</v>
-      </c>
-      <c r="CY30" s="5">
-        <f t="shared" si="36"/>
-        <v>21142.912691971502</v>
-      </c>
-      <c r="CZ30" s="5">
-        <f t="shared" si="36"/>
-        <v>21354.341818891218</v>
-      </c>
-      <c r="DA30" s="5">
-        <f t="shared" si="36"/>
-        <v>21567.885237080132</v>
-      </c>
-      <c r="DB30" s="5">
-        <f t="shared" si="36"/>
-        <v>21783.564089450934</v>
-      </c>
-      <c r="DC30" s="5">
-        <f t="shared" si="36"/>
-        <v>22001.399730345445</v>
-      </c>
-      <c r="DD30" s="5">
-        <f t="shared" si="36"/>
-        <v>22221.413727648898</v>
-      </c>
-      <c r="DE30" s="5">
-        <f t="shared" ref="DE30:EV30" si="37">+DD30*(1+$AU$36)</f>
-        <v>22443.627864925387</v>
-      </c>
-      <c r="DF30" s="5">
-        <f t="shared" si="37"/>
-        <v>22668.06414357464</v>
-      </c>
-      <c r="DG30" s="5">
-        <f t="shared" si="37"/>
-        <v>22894.744785010385</v>
-      </c>
-      <c r="DH30" s="5">
-        <f t="shared" si="37"/>
-        <v>23123.692232860489</v>
-      </c>
-      <c r="DI30" s="5">
-        <f t="shared" si="37"/>
-        <v>23354.929155189093</v>
-      </c>
-      <c r="DJ30" s="5">
-        <f t="shared" si="37"/>
-        <v>23588.478446740985</v>
-      </c>
-      <c r="DK30" s="5">
-        <f t="shared" si="37"/>
-        <v>23824.363231208394</v>
-      </c>
-      <c r="DL30" s="5">
-        <f t="shared" si="37"/>
-        <v>24062.606863520479</v>
-      </c>
-      <c r="DM30" s="5">
-        <f t="shared" si="37"/>
-        <v>24303.232932155683</v>
-      </c>
-      <c r="DN30" s="5">
-        <f t="shared" si="37"/>
-        <v>24546.265261477241</v>
-      </c>
-      <c r="DO30" s="5">
-        <f t="shared" si="37"/>
-        <v>24791.727914092015</v>
-      </c>
-      <c r="DP30" s="5">
-        <f t="shared" si="37"/>
-        <v>25039.645193232936</v>
-      </c>
-      <c r="DQ30" s="5">
-        <f t="shared" si="37"/>
-        <v>25290.041645165267</v>
-      </c>
-      <c r="DR30" s="5">
-        <f t="shared" si="37"/>
-        <v>25542.942061616919</v>
-      </c>
-      <c r="DS30" s="5">
-        <f t="shared" si="37"/>
-        <v>25798.371482233088</v>
-      </c>
-      <c r="DT30" s="5">
-        <f t="shared" si="37"/>
-        <v>26056.355197055418</v>
-      </c>
-      <c r="DU30" s="5">
-        <f t="shared" si="37"/>
-        <v>26316.918749025972</v>
-      </c>
-      <c r="DV30" s="5">
-        <f t="shared" si="37"/>
-        <v>26580.087936516233</v>
-      </c>
-      <c r="DW30" s="5">
-        <f t="shared" si="37"/>
-        <v>26845.888815881397</v>
-      </c>
-      <c r="DX30" s="5">
-        <f t="shared" si="37"/>
-        <v>27114.34770404021</v>
-      </c>
-      <c r="DY30" s="5">
-        <f t="shared" si="37"/>
-        <v>27385.491181080612</v>
-      </c>
-      <c r="DZ30" s="5">
-        <f t="shared" si="37"/>
-        <v>27659.346092891417</v>
-      </c>
-      <c r="EA30" s="5">
-        <f t="shared" si="37"/>
-        <v>27935.939553820332</v>
-      </c>
-      <c r="EB30" s="5">
-        <f t="shared" si="37"/>
-        <v>28215.298949358534</v>
-      </c>
-      <c r="EC30" s="5">
-        <f t="shared" si="37"/>
-        <v>28497.451938852118</v>
-      </c>
-      <c r="ED30" s="5">
-        <f t="shared" si="37"/>
-        <v>28782.426458240639</v>
-      </c>
-      <c r="EE30" s="5">
-        <f t="shared" si="37"/>
-        <v>29070.250722823046</v>
-      </c>
-      <c r="EF30" s="5">
-        <f t="shared" si="37"/>
-        <v>29360.953230051276</v>
-      </c>
-      <c r="EG30" s="5">
-        <f t="shared" si="37"/>
-        <v>29654.56276235179</v>
-      </c>
-      <c r="EH30" s="5">
-        <f t="shared" si="37"/>
-        <v>29951.10838997531</v>
-      </c>
-      <c r="EI30" s="5">
-        <f t="shared" si="37"/>
-        <v>30250.619473875064</v>
-      </c>
-      <c r="EJ30" s="5">
-        <f t="shared" si="37"/>
-        <v>30553.125668613815</v>
-      </c>
-      <c r="EK30" s="5">
-        <f t="shared" si="37"/>
-        <v>30858.656925299954</v>
-      </c>
-      <c r="EL30" s="5">
-        <f t="shared" si="37"/>
-        <v>31167.243494552953</v>
-      </c>
-      <c r="EM30" s="5">
-        <f t="shared" si="37"/>
-        <v>31478.915929498482</v>
-      </c>
-      <c r="EN30" s="5">
-        <f t="shared" si="37"/>
-        <v>31793.705088793467</v>
-      </c>
-      <c r="EO30" s="5">
-        <f t="shared" si="37"/>
-        <v>32111.642139681404</v>
-      </c>
-      <c r="EP30" s="5">
-        <f t="shared" si="37"/>
-        <v>32432.758561078219</v>
-      </c>
-      <c r="EQ30" s="5">
-        <f t="shared" si="37"/>
-        <v>32757.086146689002</v>
-      </c>
-      <c r="ER30" s="5">
-        <f t="shared" si="37"/>
         <v>33084.657008155889</v>
       </c>
       <c r="ES30" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="34"/>
         <v>33415.503578237447</v>
       </c>
       <c r="ET30" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="34"/>
         <v>33749.65861401982</v>
       </c>
       <c r="EU30" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="34"/>
         <v>34087.155200160021</v>
       </c>
       <c r="EV30" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="34"/>
         <v>34428.026752161619</v>
       </c>
     </row>
@@ -6081,35 +6283,35 @@
         <v>752.50226242219844</v>
       </c>
       <c r="AJ31" s="3">
-        <f t="shared" ref="AJ31:AQ31" si="38">+AI31</f>
+        <f t="shared" ref="AJ31:AQ31" si="35">+AI31</f>
         <v>752.50226242219844</v>
       </c>
       <c r="AK31" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="35"/>
         <v>752.50226242219844</v>
       </c>
       <c r="AL31" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="35"/>
         <v>752.50226242219844</v>
       </c>
       <c r="AM31" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="35"/>
         <v>752.50226242219844</v>
       </c>
       <c r="AN31" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="35"/>
         <v>752.50226242219844</v>
       </c>
       <c r="AO31" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="35"/>
         <v>752.50226242219844</v>
       </c>
       <c r="AP31" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="35"/>
         <v>752.50226242219844</v>
       </c>
       <c r="AQ31" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="35"/>
         <v>752.50226242219844</v>
       </c>
     </row>
@@ -6130,7 +6332,7 @@
         <v>1.9232558139534883</v>
       </c>
       <c r="F32" s="6">
-        <f t="shared" si="1"/>
+        <f>+AD32-SUM(C32:E32)</f>
         <v>2.3531633692905682</v>
       </c>
       <c r="G32" s="6">
@@ -6146,7 +6348,7 @@
         <v>2.1221281741233375</v>
       </c>
       <c r="J32" s="6">
-        <f t="shared" si="2"/>
+        <f>+AE32-SUM(G32:I32)</f>
         <v>1.9964691580258584</v>
       </c>
       <c r="K32" s="6">
@@ -6162,7 +6364,7 @@
         <v>1.332919254658385</v>
       </c>
       <c r="N32" s="6">
-        <f t="shared" si="3"/>
+        <f>+AF32-SUM(K32:M32)</f>
         <v>1.7831963299361546</v>
       </c>
       <c r="O32" s="6">
@@ -6178,7 +6380,7 @@
         <v>2.3202033036848793</v>
       </c>
       <c r="R32" s="6">
-        <f t="shared" si="4"/>
+        <f>+AG32-SUM(O32:Q32)</f>
         <v>2.2630380582769893</v>
       </c>
       <c r="S32" s="6">
@@ -6199,75 +6401,75 @@
       </c>
       <c r="X32" s="21"/>
       <c r="Z32" s="3">
-        <f t="shared" ref="Z32:AI32" si="39">+Z30/Z31</f>
+        <f t="shared" ref="Z32:AI32" si="36">+Z30/Z31</f>
         <v>5.5994291151284488</v>
       </c>
       <c r="AA32" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>5.1475573280159521</v>
       </c>
       <c r="AB32" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>5.7486631016042784</v>
       </c>
       <c r="AC32" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>3.1015801354401806</v>
       </c>
       <c r="AD32" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>8.0570430733410952</v>
       </c>
       <c r="AE32" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>8.1433734939759042</v>
       </c>
       <c r="AF32" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>3.8895781637717119</v>
       </c>
       <c r="AG32" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>10.20253164556962</v>
       </c>
       <c r="AH32" s="6">
-        <f t="shared" si="6"/>
+        <f>+SUM(S32:V32)</f>
         <v>10.271221406872941</v>
       </c>
       <c r="AI32" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="36"/>
         <v>10.467914985921338</v>
       </c>
       <c r="AJ32" s="6">
-        <f t="shared" ref="AJ32:AQ32" si="40">+AJ30/AJ31</f>
+        <f t="shared" ref="AJ32:AQ32" si="37">+AJ30/AJ31</f>
         <v>10.991310735217409</v>
       </c>
       <c r="AK32" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="37"/>
         <v>11.540876271978275</v>
       </c>
       <c r="AL32" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="37"/>
         <v>12.117920085577193</v>
       </c>
       <c r="AM32" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="37"/>
         <v>12.723816089856061</v>
       </c>
       <c r="AN32" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="37"/>
         <v>13.36000689434886</v>
       </c>
       <c r="AO32" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="37"/>
         <v>14.028007239066302</v>
       </c>
       <c r="AP32" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="37"/>
         <v>14.729407601019616</v>
       </c>
       <c r="AQ32" s="6">
-        <f t="shared" si="40"/>
+        <f t="shared" si="37"/>
         <v>15.465877981070603</v>
       </c>
     </row>
@@ -6280,101 +6482,101 @@
         <v>124</v>
       </c>
       <c r="G35" s="18">
-        <f t="shared" ref="G35" si="41">+G16/C16-1</f>
+        <f t="shared" ref="G35:V35" si="38">+G16/C16-1</f>
         <v>6.6474583247581709E-2</v>
       </c>
       <c r="H35" s="18">
-        <f t="shared" ref="H35" si="42">+H16/D16-1</f>
+        <f t="shared" si="38"/>
         <v>8.3583283343331427E-2</v>
       </c>
       <c r="I35" s="18">
-        <f t="shared" ref="I35" si="43">+I16/E16-1</f>
+        <f t="shared" si="38"/>
         <v>8.3300473186119772E-2</v>
       </c>
       <c r="J35" s="18">
-        <f t="shared" ref="J35" si="44">+J16/F16-1</f>
+        <f t="shared" si="38"/>
         <v>8.5067786900897557E-2</v>
       </c>
       <c r="K35" s="18">
-        <f t="shared" ref="K35" si="45">+K16/G16-1</f>
+        <f t="shared" si="38"/>
         <v>-5.2103434967194495E-3</v>
       </c>
       <c r="L35" s="18">
-        <f t="shared" ref="L35" si="46">+L16/H16-1</f>
+        <f t="shared" si="38"/>
         <v>-0.29184351356338811</v>
       </c>
       <c r="M35" s="18">
-        <f t="shared" ref="M35" si="47">+M16/I16-1</f>
+        <f t="shared" si="38"/>
         <v>-0.20365820365820364</v>
       </c>
       <c r="N35" s="18">
-        <f t="shared" ref="N35:T35" si="48">+N16/J16-1</f>
+        <f t="shared" si="38"/>
         <v>-0.17721073471183457</v>
       </c>
       <c r="O35" s="18">
-        <f t="shared" si="48"/>
+        <f t="shared" si="38"/>
         <v>-0.12085354025218231</v>
       </c>
       <c r="P35" s="18">
-        <f t="shared" si="48"/>
+        <f t="shared" si="38"/>
         <v>0.33459283387622141</v>
       </c>
       <c r="Q35" s="18">
-        <f t="shared" si="48"/>
+        <f t="shared" si="38"/>
         <v>0.24877156896354702</v>
       </c>
       <c r="R35" s="18">
-        <f>+R16/N16-1</f>
+        <f t="shared" si="38"/>
         <v>0.29879157309378668</v>
       </c>
       <c r="S35" s="18">
-        <f t="shared" si="48"/>
+        <f t="shared" si="38"/>
         <v>0.29666813768755507</v>
       </c>
       <c r="T35" s="18">
-        <f t="shared" si="48"/>
+        <f t="shared" si="38"/>
         <v>0.30772234696866163</v>
       </c>
       <c r="U35" s="18">
-        <f>+U16/O16-1</f>
-        <v>0.49558693733451009</v>
+        <f t="shared" si="38"/>
+        <v>0.24048316251830171</v>
       </c>
       <c r="V35" s="18">
-        <f>+V16/P16-1</f>
-        <v>0.22209919755195595</v>
+        <f t="shared" si="38"/>
+        <v>3.0709105024675498E-2</v>
       </c>
       <c r="X35" s="15"/>
       <c r="Z35" s="5"/>
       <c r="AA35" s="18">
-        <f t="shared" ref="AA35:AE35" si="49">+AA16/Z16-1</f>
+        <f t="shared" ref="AA35:AH35" si="39">+AA16/Z16-1</f>
         <v>-4.0072540072540019E-2</v>
       </c>
       <c r="AB35" s="18">
-        <f t="shared" si="49"/>
+        <f t="shared" si="39"/>
         <v>7.9834237308793909E-2</v>
       </c>
       <c r="AC35" s="18">
-        <f t="shared" si="49"/>
+        <f t="shared" si="39"/>
         <v>4.0634347310796404E-2</v>
       </c>
       <c r="AD35" s="18">
-        <f t="shared" si="49"/>
+        <f t="shared" si="39"/>
         <v>9.3822875427084007E-2</v>
       </c>
       <c r="AE35" s="18">
-        <f t="shared" si="49"/>
+        <f t="shared" si="39"/>
         <v>7.9775893698249778E-2</v>
       </c>
       <c r="AF35" s="18">
-        <f>+AF16/AE16-1</f>
+        <f t="shared" si="39"/>
         <v>-0.17148039305721374</v>
       </c>
       <c r="AG35" s="18">
-        <f t="shared" ref="AG35:AH35" si="50">+AG16/AF16-1</f>
+        <f t="shared" si="39"/>
         <v>0.17438412724803953</v>
       </c>
       <c r="AH35" s="18">
-        <f t="shared" si="50"/>
+        <f t="shared" si="39"/>
         <v>0.20863525437764707</v>
       </c>
       <c r="AI35" s="18">
@@ -6468,31 +6670,31 @@
         <v>-11865</v>
       </c>
       <c r="O38" s="3">
-        <f t="shared" ref="O38:U38" si="51">+O42-O53-O54</f>
+        <f t="shared" ref="O38:U38" si="40">+O42-O53-O54</f>
         <v>-3317</v>
       </c>
       <c r="P38" s="3">
-        <f t="shared" si="51"/>
+        <f t="shared" si="40"/>
         <v>-8431</v>
       </c>
       <c r="Q38" s="3">
-        <f t="shared" si="51"/>
+        <f t="shared" si="40"/>
         <v>-8820</v>
       </c>
       <c r="R38" s="3">
-        <f t="shared" si="51"/>
+        <f t="shared" si="40"/>
         <v>-18890</v>
       </c>
       <c r="S38" s="3">
-        <f t="shared" si="51"/>
+        <f t="shared" si="40"/>
         <v>-12781</v>
       </c>
       <c r="T38" s="3">
-        <f t="shared" si="51"/>
+        <f t="shared" si="40"/>
         <v>-16202</v>
       </c>
       <c r="U38" s="3">
-        <f t="shared" si="51"/>
+        <f t="shared" si="40"/>
         <v>-12726</v>
       </c>
       <c r="AS38" s="10"/>
@@ -6504,31 +6706,31 @@
         <v>139331.23651756116</v>
       </c>
       <c r="AV38" s="29">
-        <f>NPV(AV37,$AH$30:$EV$30)</f>
+        <f t="shared" ref="AV38:BB38" si="41">NPV(AV37,$AH$30:$EV$30)</f>
         <v>198653.36513426161</v>
       </c>
       <c r="AW38" s="29">
-        <f>NPV(AW37,$AH$30:$EV$30)</f>
+        <f t="shared" si="41"/>
         <v>179855.18151814537</v>
       </c>
       <c r="AX38" s="29">
-        <f>NPV(AX37,$AH$30:$EV$30)</f>
+        <f t="shared" si="41"/>
         <v>164116.97941418868</v>
       </c>
       <c r="AY38" s="29">
-        <f>NPV(AY37,$AH$30:$EV$30)</f>
+        <f t="shared" si="41"/>
         <v>150773.08077482271</v>
       </c>
       <c r="AZ38" s="29">
-        <f>NPV(AZ37,$AH$30:$EV$30)</f>
+        <f t="shared" si="41"/>
         <v>120762.40277327025</v>
       </c>
       <c r="BA38" s="29">
-        <f>NPV(BA37,$AH$30:$EV$30)</f>
+        <f t="shared" si="41"/>
         <v>113135.35293184689</v>
       </c>
       <c r="BB38" s="29">
-        <f>NPV(BB37,$AH$30:$EV$30)</f>
+        <f t="shared" si="41"/>
         <v>106369.59113459302</v>
       </c>
       <c r="BC38" s="29"/>
@@ -6621,19 +6823,19 @@
         <v>185927.36513426161</v>
       </c>
       <c r="AW40" s="30">
-        <f t="shared" ref="AW40:BA40" si="52">+AW38+$AU$39</f>
+        <f t="shared" ref="AW40:AZ40" si="42">+AW38+$AU$39</f>
         <v>167129.18151814537</v>
       </c>
       <c r="AX40" s="30">
-        <f t="shared" si="52"/>
+        <f t="shared" si="42"/>
         <v>151390.97941418868</v>
       </c>
       <c r="AY40" s="30">
-        <f t="shared" si="52"/>
+        <f t="shared" si="42"/>
         <v>138047.08077482271</v>
       </c>
       <c r="AZ40" s="30">
-        <f t="shared" si="52"/>
+        <f t="shared" si="42"/>
         <v>108036.40277327025</v>
       </c>
       <c r="BA40" s="30">
@@ -6699,35 +6901,35 @@
         <v>57</v>
       </c>
       <c r="N42" s="5">
-        <f>+SUM(N39:N41)</f>
+        <f t="shared" ref="N42:U42" si="43">+SUM(N39:N41)</f>
         <v>32965</v>
       </c>
       <c r="O42" s="5">
-        <f>+SUM(O39:O41)</f>
+        <f t="shared" si="43"/>
         <v>40280</v>
       </c>
       <c r="P42" s="5">
-        <f>+SUM(P39:P41)</f>
+        <f t="shared" si="43"/>
         <v>30796</v>
       </c>
       <c r="Q42" s="5">
-        <f>+SUM(Q39:Q41)</f>
+        <f t="shared" si="43"/>
         <v>27916</v>
       </c>
       <c r="R42" s="5">
-        <f>+SUM(R39:R41)</f>
+        <f t="shared" si="43"/>
         <v>22028</v>
       </c>
       <c r="S42" s="5">
-        <f>+SUM(S39:S41)</f>
+        <f t="shared" si="43"/>
         <v>27678</v>
       </c>
       <c r="T42" s="5">
-        <f>+SUM(T39:T41)</f>
+        <f t="shared" si="43"/>
         <v>26277</v>
       </c>
       <c r="U42" s="5">
-        <f>+SUM(U39:U41)</f>
+        <f t="shared" si="43"/>
         <v>31182</v>
       </c>
       <c r="X42" s="13"/>
@@ -6740,31 +6942,31 @@
         <v>169.4321423504214</v>
       </c>
       <c r="AV42" s="31">
-        <f>+AV40/$AU$41</f>
+        <f t="shared" ref="AV42:BB42" si="44">+AV40/$AU$41</f>
         <v>248.82123885845274</v>
       </c>
       <c r="AW42" s="31">
-        <f t="shared" ref="AW42:BA42" si="53">+AW40/$AU$41</f>
+        <f t="shared" si="44"/>
         <v>223.66417103106173</v>
       </c>
       <c r="AX42" s="31">
-        <f t="shared" si="53"/>
+        <f t="shared" si="44"/>
         <v>202.60218834721422</v>
       </c>
       <c r="AY42" s="31">
-        <f t="shared" si="53"/>
+        <f t="shared" si="44"/>
         <v>184.74443304448593</v>
       </c>
       <c r="AZ42" s="31">
-        <f t="shared" si="53"/>
+        <f t="shared" si="44"/>
         <v>144.58200685221388</v>
       </c>
       <c r="BA42" s="31">
-        <f>+BA40/$AU$41</f>
+        <f t="shared" si="44"/>
         <v>134.37494567535211</v>
       </c>
       <c r="BB42" s="31">
-        <f>+BB40/$AU$41</f>
+        <f t="shared" si="44"/>
         <v>125.3205214866468</v>
       </c>
       <c r="BC42" s="32"/>
@@ -7053,35 +7255,35 @@
         <v>63</v>
       </c>
       <c r="N49" s="5">
-        <f>+SUM(N42:N48)</f>
+        <f t="shared" ref="N49:U49" si="45">+SUM(N42:N48)</f>
         <v>191367</v>
       </c>
       <c r="O49" s="5">
-        <f>+SUM(O42:O48)</f>
+        <f t="shared" si="45"/>
         <v>193067</v>
       </c>
       <c r="P49" s="5">
-        <f>+SUM(P42:P48)</f>
+        <f t="shared" si="45"/>
         <v>186973</v>
       </c>
       <c r="Q49" s="5">
-        <f>+SUM(Q42:Q48)</f>
+        <f t="shared" si="45"/>
         <v>184261</v>
       </c>
       <c r="R49" s="5">
-        <f>+SUM(R42:R48)</f>
+        <f t="shared" si="45"/>
         <v>188548</v>
       </c>
       <c r="S49" s="5">
-        <f>+SUM(S42:S48)</f>
+        <f t="shared" si="45"/>
         <v>195862</v>
       </c>
       <c r="T49" s="5">
-        <f>+SUM(T42:T48)</f>
+        <f t="shared" si="45"/>
         <v>205298</v>
       </c>
       <c r="U49" s="5">
-        <f>+SUM(U42:U48)</f>
+        <f t="shared" si="45"/>
         <v>214915</v>
       </c>
       <c r="X49" s="13"/>
@@ -7236,35 +7438,35 @@
         <v>69</v>
       </c>
       <c r="N56" s="5">
-        <f>+SUM(N51:N55)</f>
+        <f t="shared" ref="N56:U56" si="46">+SUM(N51:N55)</f>
         <v>168383</v>
       </c>
       <c r="O56" s="5">
-        <f>+SUM(O51:O55)</f>
+        <f t="shared" si="46"/>
         <v>168618</v>
       </c>
       <c r="P56" s="5">
-        <f>+SUM(P51:P55)</f>
+        <f t="shared" si="46"/>
         <v>161434</v>
       </c>
       <c r="Q56" s="5">
-        <f>+SUM(Q51:Q55)</f>
+        <f t="shared" si="46"/>
         <v>159835</v>
       </c>
       <c r="R56" s="5">
-        <f>+SUM(R51:R55)</f>
+        <f t="shared" si="46"/>
         <v>166371</v>
       </c>
       <c r="S56" s="5">
-        <f>+SUM(S51:S55)</f>
+        <f t="shared" si="46"/>
         <v>173479</v>
       </c>
       <c r="T56" s="5">
-        <f>+SUM(T51:T55)</f>
+        <f t="shared" si="46"/>
         <v>182063</v>
       </c>
       <c r="U56" s="5">
-        <f>+SUM(U51:U55)</f>
+        <f t="shared" si="46"/>
         <v>190975</v>
       </c>
       <c r="X56" s="13"/>
@@ -7481,19 +7683,19 @@
         <v>-2895</v>
       </c>
       <c r="O64" s="3">
-        <f t="shared" ref="O64:R64" si="54">+SUM(O61:O63)</f>
+        <f t="shared" ref="O64:R64" si="47">+SUM(O61:O63)</f>
         <v>-2898</v>
       </c>
       <c r="P64" s="3">
-        <f t="shared" si="54"/>
+        <f t="shared" si="47"/>
         <v>-2881</v>
       </c>
       <c r="Q64" s="3">
-        <f t="shared" si="54"/>
+        <f t="shared" si="47"/>
         <v>-2963</v>
       </c>
       <c r="R64" s="3">
-        <f t="shared" si="54"/>
+        <f t="shared" si="47"/>
         <v>-2945</v>
       </c>
       <c r="S64" s="3">
@@ -7548,35 +7750,35 @@
         <v>54</v>
       </c>
       <c r="N66" s="5">
-        <f>+N56+N65</f>
+        <f t="shared" ref="N66:U66" si="48">+N56+N65</f>
         <v>191367</v>
       </c>
       <c r="O66" s="5">
-        <f>+O56+O65</f>
+        <f t="shared" si="48"/>
         <v>193067</v>
       </c>
       <c r="P66" s="5">
-        <f>+P56+P65</f>
+        <f t="shared" si="48"/>
         <v>186973</v>
       </c>
       <c r="Q66" s="5">
-        <f>+Q56+Q65</f>
+        <f t="shared" si="48"/>
         <v>184261</v>
       </c>
       <c r="R66" s="5">
-        <f>+R56+R65</f>
+        <f t="shared" si="48"/>
         <v>188548</v>
       </c>
       <c r="S66" s="5">
-        <f>+S56+S65</f>
+        <f t="shared" si="48"/>
         <v>195862</v>
       </c>
       <c r="T66" s="5">
-        <f>+T56+T65</f>
+        <f t="shared" si="48"/>
         <v>205298</v>
       </c>
       <c r="U66" s="5">
-        <f>+U56+U65</f>
+        <f t="shared" si="48"/>
         <v>214915</v>
       </c>
       <c r="X66" s="13"/>
@@ -7692,35 +7894,35 @@
         <v>81</v>
       </c>
       <c r="N72" s="7">
-        <f>SUM(K30:N30)/N65</f>
+        <f t="shared" ref="N72:U72" si="49">SUM(K30:N30)/N65</f>
         <v>0.13639923424991299</v>
       </c>
       <c r="O72" s="7">
-        <f>SUM(L30:O30)/O65</f>
+        <f t="shared" si="49"/>
         <v>0.20463004621865924</v>
       </c>
       <c r="P72" s="7">
-        <f>SUM(M30:P30)/P65</f>
+        <f t="shared" si="49"/>
         <v>0.27510865734758605</v>
       </c>
       <c r="Q72" s="7">
-        <f>SUM(N30:Q30)/Q65</f>
+        <f t="shared" si="49"/>
         <v>0.31847211987226726</v>
       </c>
       <c r="R72" s="7">
-        <f>SUM(O30:R30)/R65</f>
+        <f t="shared" si="49"/>
         <v>0.36343959958515581</v>
       </c>
       <c r="S72" s="7">
-        <f>SUM(P30:S30)/S65</f>
+        <f t="shared" si="49"/>
         <v>0.35634186659518385</v>
       </c>
       <c r="T72" s="7">
-        <f>SUM(Q30:T30)/T65</f>
+        <f t="shared" si="49"/>
         <v>0.3296750591779643</v>
       </c>
       <c r="U72" s="7">
-        <f>SUM(R30:U30)/U65</f>
+        <f t="shared" si="49"/>
         <v>0.32218045112781957</v>
       </c>
       <c r="X72" s="14"/>
@@ -7731,35 +7933,35 @@
         <v>83</v>
       </c>
       <c r="N73" s="3">
-        <f>+N49-N56</f>
+        <f t="shared" ref="N73:U73" si="50">+N49-N56</f>
         <v>22984</v>
       </c>
       <c r="O73" s="3">
-        <f>+O49-O56</f>
+        <f t="shared" si="50"/>
         <v>24449</v>
       </c>
       <c r="P73" s="3">
-        <f>+P49-P56</f>
+        <f t="shared" si="50"/>
         <v>25539</v>
       </c>
       <c r="Q73" s="3">
-        <f>+Q49-Q56</f>
+        <f t="shared" si="50"/>
         <v>24426</v>
       </c>
       <c r="R73" s="3">
-        <f>+R49-R56</f>
+        <f t="shared" si="50"/>
         <v>22177</v>
       </c>
       <c r="S73" s="3">
-        <f>+S49-S56</f>
+        <f t="shared" si="50"/>
         <v>22383</v>
       </c>
       <c r="T73" s="3">
-        <f>+T49-T56</f>
+        <f t="shared" si="50"/>
         <v>23235</v>
       </c>
       <c r="U73" s="3">
-        <f>+U49-U56</f>
+        <f t="shared" si="50"/>
         <v>23940</v>
       </c>
     </row>
@@ -8048,31 +8250,31 @@
         <v>91</v>
       </c>
       <c r="O85" s="5">
-        <f>+SUM(O75:O84)</f>
+        <f t="shared" ref="O85:U85" si="51">+SUM(O75:O84)</f>
         <v>2280</v>
       </c>
       <c r="P85" s="5">
-        <f>+SUM(P75:P84)</f>
+        <f t="shared" si="51"/>
         <v>3185</v>
       </c>
       <c r="Q85" s="5">
-        <f>+SUM(Q75:Q84)</f>
+        <f t="shared" si="51"/>
         <v>4172</v>
       </c>
       <c r="R85" s="5">
-        <f>+SUM(R75:R84)</f>
+        <f t="shared" si="51"/>
         <v>5008</v>
       </c>
       <c r="S85" s="5">
-        <f>+SUM(S75:S84)</f>
+        <f t="shared" si="51"/>
         <v>3880</v>
       </c>
       <c r="T85" s="5">
-        <f>+SUM(T75:T84)</f>
+        <f t="shared" si="51"/>
         <v>4259</v>
       </c>
       <c r="U85" s="5">
-        <f>+SUM(U75:U84)</f>
+        <f t="shared" si="51"/>
         <v>4508</v>
       </c>
       <c r="X85" s="13"/>
@@ -8297,31 +8499,31 @@
         <v>99</v>
       </c>
       <c r="O94" s="5">
-        <f>+SUM(O87:O93)</f>
+        <f t="shared" ref="O94:U94" si="52">+SUM(O87:O93)</f>
         <v>4774</v>
       </c>
       <c r="P94" s="5">
-        <f>+SUM(P87:P93)</f>
+        <f t="shared" si="52"/>
         <v>-2765</v>
       </c>
       <c r="Q94" s="5">
-        <f>+SUM(Q87:Q93)</f>
+        <f t="shared" si="52"/>
         <v>-1216</v>
       </c>
       <c r="R94" s="5">
-        <f>+SUM(R87:R93)</f>
+        <f t="shared" si="52"/>
         <v>-11322</v>
       </c>
       <c r="S94" s="5">
-        <f>+SUM(S87:S93)</f>
+        <f t="shared" si="52"/>
         <v>-2777</v>
       </c>
       <c r="T94" s="5">
-        <f>+SUM(T87:T93)</f>
+        <f t="shared" si="52"/>
         <v>-12615</v>
       </c>
       <c r="U94" s="5">
-        <f>+SUM(U87:U93)</f>
+        <f t="shared" si="52"/>
         <v>-7523</v>
       </c>
       <c r="X94" s="13"/>
@@ -8606,31 +8808,31 @@
         <v>107</v>
       </c>
       <c r="O105" s="5">
-        <f>+SUM(O96:O104)</f>
+        <f t="shared" ref="O105:U105" si="53">+SUM(O96:O104)</f>
         <v>461</v>
       </c>
       <c r="P105" s="5">
-        <f>+SUM(P96:P104)</f>
+        <f t="shared" si="53"/>
         <v>-9877</v>
       </c>
       <c r="Q105" s="5">
-        <f>+SUM(Q96:Q104)</f>
+        <f t="shared" si="53"/>
         <v>-5882</v>
       </c>
       <c r="R105" s="5">
-        <f>+SUM(R96:R104)</f>
+        <f t="shared" si="53"/>
         <v>365</v>
       </c>
       <c r="S105" s="5">
-        <f>+SUM(S96:S104)</f>
+        <f t="shared" si="53"/>
         <v>4533</v>
       </c>
       <c r="T105" s="5">
-        <f>+SUM(T96:T104)</f>
+        <f t="shared" si="53"/>
         <v>5868</v>
       </c>
       <c r="U105" s="5">
-        <f>+SUM(U96:U104)</f>
+        <f t="shared" si="53"/>
         <v>8532</v>
       </c>
       <c r="W105" s="3"/>
@@ -8673,31 +8875,31 @@
         <v>109</v>
       </c>
       <c r="O107" s="5">
-        <f>+O85+O94+O105+O106</f>
+        <f t="shared" ref="O107:U107" si="54">+O85+O94+O105+O106</f>
         <v>7315</v>
       </c>
       <c r="P107" s="5">
-        <f>+P85+P94+P105+P106</f>
+        <f t="shared" si="54"/>
         <v>-9484</v>
       </c>
       <c r="Q107" s="5">
-        <f>+Q85+Q94+Q105+Q106</f>
+        <f t="shared" si="54"/>
         <v>-2880</v>
       </c>
       <c r="R107" s="5">
-        <f>+R85+R94+R105+R106</f>
+        <f t="shared" si="54"/>
         <v>-5888</v>
       </c>
       <c r="S107" s="5">
-        <f>+S85+S94+S105+S106</f>
+        <f t="shared" si="54"/>
         <v>5650</v>
       </c>
       <c r="T107" s="5">
-        <f>+T85+T94+T105+T106</f>
+        <f t="shared" si="54"/>
         <v>-2218</v>
       </c>
       <c r="U107" s="5">
-        <f>+U85+U94+U105+U106</f>
+        <f t="shared" si="54"/>
         <v>5722</v>
       </c>
       <c r="W107" s="3"/>
@@ -8750,15 +8952,15 @@
         <v>2875</v>
       </c>
       <c r="Q110" s="3">
-        <f t="shared" si="56"/>
+        <f>+Q109-Q77</f>
         <v>2710</v>
       </c>
       <c r="R110" s="3">
-        <f t="shared" si="56"/>
+        <f>+R109-R77</f>
         <v>4044</v>
       </c>
       <c r="S110" s="3">
-        <f t="shared" si="56"/>
+        <f>+S109-S77</f>
         <v>2913</v>
       </c>
       <c r="T110" s="3">
@@ -8879,10 +9081,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF9450D-0D90-A549-B47E-BDB7BA4F058F}">
-  <dimension ref="B3:J36"/>
+  <dimension ref="B3:M36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -8892,12 +9094,12 @@
     <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.5" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:13">
       <c r="B3" t="s">
         <v>127</v>
       </c>
@@ -8905,7 +9107,7 @@
         <v>1850</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:13">
       <c r="B4" t="s">
         <v>171</v>
       </c>
@@ -8917,7 +9119,7 @@
       </c>
       <c r="G4" s="50"/>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:13">
       <c r="E5" s="51" t="s">
         <v>13</v>
       </c>
@@ -8927,8 +9129,13 @@
       <c r="G5" s="53" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="6" spans="2:7">
+      <c r="J5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="57" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
       <c r="B6" s="23" t="s">
         <v>128</v>
       </c>
@@ -8941,7 +9148,7 @@
       </c>
       <c r="G6" s="53"/>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:13">
       <c r="B7" t="s">
         <v>129</v>
       </c>
@@ -8959,7 +9166,7 @@
         <v>Q322</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:13">
       <c r="B8" t="s">
         <v>130</v>
       </c>
@@ -8978,7 +9185,7 @@
         <v>Q322</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:13">
       <c r="B9" t="s">
         <v>131</v>
       </c>
@@ -8994,39 +9201,71 @@
       </c>
       <c r="G9" s="56"/>
     </row>
-    <row r="12" spans="2:7">
+    <row r="11" spans="2:13">
+      <c r="F11" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
       <c r="B12" s="23" t="s">
         <v>134</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="13" spans="2:7">
+      <c r="F12" t="s">
+        <v>185</v>
+      </c>
+      <c r="K12" s="58" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
       <c r="B13" t="s">
         <v>135</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="14" spans="2:7">
+      <c r="F13" t="s">
+        <v>186</v>
+      </c>
+      <c r="K13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
       <c r="B14" t="s">
         <v>136</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="15" spans="2:7">
+      <c r="F14" t="s">
+        <v>187</v>
+      </c>
+      <c r="K14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
       <c r="B15" t="s">
         <v>137</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="16" spans="2:7">
+      <c r="F15" t="s">
+        <v>184</v>
+      </c>
+      <c r="K15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
       <c r="B16" t="s">
         <v>138</v>
       </c>
@@ -9034,12 +9273,12 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:8">
       <c r="C17" s="26" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:8">
       <c r="B18" s="22" t="s">
         <v>142</v>
       </c>
@@ -9047,31 +9286,46 @@
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:8">
       <c r="B19" t="s">
         <v>143</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="20" spans="2:3">
+      <c r="F19" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
       <c r="B20" t="s">
         <v>144</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="21" spans="2:3">
+      <c r="F20" s="60">
+        <v>44861</v>
+      </c>
+      <c r="H20" s="61">
+        <v>44875</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
       <c r="B21" t="s">
         <v>145</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="22" spans="2:3">
+      <c r="F21" s="59">
+        <v>44895</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
       <c r="B22" t="s">
         <v>146</v>
       </c>
@@ -9079,7 +9333,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:8">
       <c r="B23" t="s">
         <v>147</v>
       </c>
@@ -9087,47 +9341,47 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:8">
       <c r="B24" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:8">
       <c r="B25" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:8">
       <c r="B26" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:8">
       <c r="B27" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:8">
       <c r="B28" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:8">
       <c r="B29" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:8">
       <c r="B30" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:8">
       <c r="B31" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:8">
       <c r="B32" t="s">
         <v>156</v>
       </c>
@@ -9166,8 +9420,25 @@
     <hyperlink ref="C21" r:id="rId10" xr:uid="{BE8186D6-9485-5E4F-957C-1B472DCFA6E1}"/>
     <hyperlink ref="C22" r:id="rId11" xr:uid="{285FA3F0-F602-5348-B259-9DA29BBF2B53}"/>
     <hyperlink ref="C23" r:id="rId12" xr:uid="{FAC94E8F-F76B-1042-9291-5BC48C55B6B4}"/>
+    <hyperlink ref="F20" r:id="rId13" display="https://www.bea.gov/news/2022/gross-domestic-product-third-quarter-2022-advance-estimate" xr:uid="{51A6DF85-DD92-E34B-9E07-03740C18E937}"/>
+    <hyperlink ref="H20" r:id="rId14" display="https://www.federalreserve.gov/releases/h41/20221110/" xr:uid="{8AB4336E-7D16-3E4A-A4F4-ABEEA1CB4B2A}"/>
+    <hyperlink ref="H19" r:id="rId15" xr:uid="{0D0D0CD9-12A6-F846-AE22-538597E9B57B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId13"/>
+  <legacyDrawing r:id="rId16"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49E8F20-701C-834E-8549-DD0249DDA890}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="242" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>